<commit_message>
new types of code checks: forbidden, regexes
</commit_message>
<xml_diff>
--- a/src/app/admin/adminUtils/tests.xlsx
+++ b/src/app/admin/adminUtils/tests.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dayfireacad/trainpython/src/admin/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dayfireacad/trainpython/src/app/admin/adminUtils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AAFEAD-1156-5F47-A795-0DF29789490B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C3DCF1-6895-8E49-A047-839EE2F87534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{A1EC0760-0569-1443-8C4C-047456B792FA}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
   <si>
     <t>task</t>
   </si>
@@ -188,13 +188,31 @@
   </si>
   <si>
     <t>a=input()\nprint(int(a/3))</t>
+  </si>
+  <si>
+    <t>forbidden</t>
+  </si>
+  <si>
+    <t>[[].*for.*in.*];[[].*for.*in.*]</t>
+  </si>
+  <si>
+    <t>musthavere</t>
+  </si>
+  <si>
+    <t>forbiddenre</t>
+  </si>
+  <si>
+    <t>+;[</t>
+  </si>
+  <si>
+    <t>[[].*?];[[].*?]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -223,6 +241,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -241,10 +267,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -258,8 +285,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -572,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3359BBA2-D3CF-9A4D-8F52-F9BD733F6E43}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -585,13 +619,15 @@
     <col min="5" max="5" width="17.6640625" style="1" customWidth="1"/>
     <col min="6" max="7" width="89.5" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="10.83203125" style="1"/>
-    <col min="10" max="10" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.1640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -620,19 +656,28 @@
         <v>4</v>
       </c>
       <c r="J1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -660,20 +705,26 @@
       <c r="I2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -702,20 +753,20 @@
       <c r="I3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="1">
+      <c r="M3" s="1">
         <v>19</v>
       </c>
-      <c r="K3" s="1">
+      <c r="N3" s="1">
         <v>6</v>
       </c>
-      <c r="L3" s="1">
+      <c r="O3" s="1">
         <v>20</v>
       </c>
-      <c r="M3" s="1">
+      <c r="P3" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ref="A4:A7" si="0">A3+1</f>
         <v>3</v>
@@ -738,17 +789,17 @@
       <c r="H4" s="1">
         <v>2</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="J4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -777,20 +828,20 @@
       <c r="I5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -819,20 +870,20 @@
       <c r="I6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="1">
+      <c r="N6" s="1">
         <v>7</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M6" s="1">
+      <c r="P6" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -858,15 +909,15 @@
       <c r="I7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L7" s="3"/>
-      <c r="M7" s="1" t="s">
+      <c r="O7" s="3"/>
+      <c r="P7" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" ref="A8" si="1">A7+1</f>
         <v>7</v>
@@ -892,15 +943,15 @@
       <c r="I8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L8" s="3"/>
-      <c r="M8" s="1" t="s">
+      <c r="O8" s="3"/>
+      <c r="P8" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" ref="A9" si="2">A8+1</f>
         <v>8</v>
@@ -926,15 +977,15 @@
       <c r="I9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="1" t="s">
+      <c r="O9" s="3"/>
+      <c r="P9" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <f>A9+1</f>
         <v>9</v>
@@ -960,15 +1011,15 @@
       <c r="I10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="1" t="s">
+      <c r="O10" s="3"/>
+      <c r="P10" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" ref="A11:A16" si="3">A10+1</f>
         <v>10</v>
@@ -976,9 +1027,9 @@
       <c r="B11">
         <v>3</v>
       </c>
-      <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="3"/>
         <v>11</v>
@@ -986,9 +1037,9 @@
       <c r="B12">
         <v>3</v>
       </c>
-      <c r="L12" s="3"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="3"/>
         <v>12</v>
@@ -996,9 +1047,9 @@
       <c r="B13">
         <v>3</v>
       </c>
-      <c r="L13" s="3"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="3"/>
         <v>13</v>
@@ -1006,9 +1057,9 @@
       <c r="B14">
         <v>3</v>
       </c>
-      <c r="L14" s="3"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O14" s="3"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="3"/>
         <v>14</v>
@@ -1016,9 +1067,9 @@
       <c r="B15">
         <v>3</v>
       </c>
-      <c r="L15" s="3"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="3"/>
         <v>15</v>
@@ -1028,6 +1079,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" display="\\[.*?\\];\\[.*?\\]" xr:uid="{DCA2EB90-B730-EE4E-9EFC-1E8EC739C87D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>